<commit_message>
Rotated U1 to fit in place properly
</commit_message>
<xml_diff>
--- a/cam/DCDC-12V5V1A_2023-06-18-PnP.xlsx
+++ b/cam/DCDC-12V5V1A_2023-06-18-PnP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\DC-DC\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5049EC83-E870-4FFF-9231-B06BD06390BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6FD9F3-1DD9-4C51-AECF-66B14C4DB2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1428" yWindow="3504" windowWidth="26388" windowHeight="20412" xr2:uid="{DE884AF9-7D55-461B-A4E3-8461E9F44E15}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="10800" windowHeight="18684" xr2:uid="{DE884AF9-7D55-461B-A4E3-8461E9F44E15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -505,7 +505,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -955,7 +955,7 @@
         <v>29</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>